<commit_message>
updated excel and json file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/demoData.xlsx
+++ b/src/test/resources/testData/demoData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccagov-my.sharepoint.com/personal/fosman_dcca_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fosman\IdeaProjects\mtf-automation-testing-api\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFEDCF16-C469-4864-89AE-E3ED5229B47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC01A6B-EFBA-4A1B-975F-B18BEF649C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="testData" sheetId="2" r:id="rId2"/>
+    <sheet name="Create" sheetId="1" r:id="rId1"/>
+    <sheet name="List users" sheetId="2" r:id="rId2"/>
+    <sheet name="Update" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,17 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>testcase</t>
   </si>
   <si>
-    <t>endpoint</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -60,17 +55,23 @@
     <t>TC1000</t>
   </si>
   <si>
-    <t>/api/users</t>
-  </si>
-  <si>
-    <t>POST</t>
+    <t>TC1001</t>
+  </si>
+  <si>
+    <t>TC1002</t>
+  </si>
+  <si>
+    <t>TC1003</t>
+  </si>
+  <si>
+    <t>updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,14 +84,6 @@
       <color rgb="FF297BDE"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,19 +103,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E585723F-DA52-4C5A-A7AB-E6B3EDE8D02A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,21 +446,26 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://reqres.in/api/users" xr:uid="{93BDDF1A-97DD-4E56-BFC4-30DEE0727B33}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -479,25 +474,57 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50213A1B-1227-4059-96C5-1D4C35B0523F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>